<commit_message>
Code refactoring for #8
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\CompositePortraitRecongnition\results\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\_MSVS_projects\teach\CompositePortraitRecongnition\results\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -15,7 +15,7 @@
     <sheet name="results" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="162913"/>
 </workbook>
 </file>
 
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -368,9 +368,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -379,7 +381,7 @@
     <col min="3" max="3" width="32.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -390,7 +392,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -400,8 +402,12 @@
       <c r="C2">
         <v>0.57948822115796694</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <f>B2/C2</f>
+        <v>1.0045220267061328</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -411,8 +417,12 @@
       <c r="C3">
         <v>0.69009060997317639</v>
       </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D3">
+        <f t="shared" ref="D3:D5" si="0">B3/C3</f>
+        <v>1.0116682053669581</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -422,8 +432,12 @@
       <c r="C4">
         <v>0.81148430201312616</v>
       </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <f t="shared" si="0"/>
+        <v>0.93570305741755877</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -432,6 +446,16 @@
       </c>
       <c r="C5">
         <v>0.6384303963590946</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="0"/>
+        <v>1.0239472126513036</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D6">
+        <f>SUM(D2:D5)/4</f>
+        <v>0.9939601255354884</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
to issue #11 added comparison tensorflow and arcface
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -414,7 +414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -430,12 +430,17 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Расстояние до переноса стиля</t>
+          <t>Расстояние до переноса стиля tensorflow</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Расстояние после переноса стиля</t>
+          <t>Расстояние после переноса стиля tensorflow</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Расстояние до переноса стиля arcface,Расстояние после переноса стиля arcface</t>
         </is>
       </c>
     </row>
@@ -449,6 +454,12 @@
       <c r="C2" t="n">
         <v>0.6900906099731764</v>
       </c>
+      <c r="D2" t="n">
+        <v>0.03230053186416626</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.01071752980351448</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -460,6 +471,12 @@
       <c r="C3" t="n">
         <v>0.8114843020131262</v>
       </c>
+      <c r="D3" t="n">
+        <v>0.07159358263015747</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.06596450507640839</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -471,6 +488,12 @@
       <c r="C4" t="n">
         <v>0.6384303963590946</v>
       </c>
+      <c r="D4" t="n">
+        <v>0.1831206232309341</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.01908320561051369</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -480,7 +503,13 @@
         <v>0.7718901967512342</v>
       </c>
       <c r="C5" t="n">
-        <v>0.7964303098175904</v>
+        <v>0.7964307258438679</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.11044642329216</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.03032833524048328</v>
       </c>
     </row>
     <row r="6">
@@ -493,6 +522,12 @@
       <c r="C6" t="n">
         <v>0.6163731154104217</v>
       </c>
+      <c r="D6" t="n">
+        <v>0.05190222710371017</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.06330510973930359</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -504,6 +539,12 @@
       <c r="C7" t="n">
         <v>0.6820363932821293</v>
       </c>
+      <c r="D7" t="n">
+        <v>0.0741061195731163</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.0427030511200428</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -515,6 +556,12 @@
       <c r="C8" t="n">
         <v>0.6573289094154495</v>
       </c>
+      <c r="D8" t="n">
+        <v>0.06903903931379318</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.04660750180482864</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -526,6 +573,12 @@
       <c r="C9" t="n">
         <v>0.5903696824065264</v>
       </c>
+      <c r="D9" t="n">
+        <v>0.05451708287000656</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.03171984478831291</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -535,7 +588,13 @@
         <v>0.7669342175270629</v>
       </c>
       <c r="C10" t="n">
-        <v>0.7330400849497321</v>
+        <v>0.7330427481233784</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.1547363102436066</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.08104228973388672</v>
       </c>
     </row>
     <row r="11">
@@ -546,7 +605,13 @@
         <v>0.7950532845299012</v>
       </c>
       <c r="C11" t="n">
-        <v>0.754820729126691</v>
+        <v>0.754825674803941</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.04635890573263168</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.06895835697650909</v>
       </c>
     </row>
     <row r="12">
@@ -557,7 +622,13 @@
         <v>0.4914829060884561</v>
       </c>
       <c r="C12" t="n">
-        <v>0.4725797102277756</v>
+        <v>0.4725813935492413</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.01744678616523743</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.02074667811393738</v>
       </c>
     </row>
     <row r="13">
@@ -570,6 +641,12 @@
       <c r="C13" t="n">
         <v>0.6552857113411387</v>
       </c>
+      <c r="D13" t="n">
+        <v>0.03705150634050369</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.02712763473391533</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -581,6 +658,12 @@
       <c r="C14" t="n">
         <v>0.7545523635001893</v>
       </c>
+      <c r="D14" t="n">
+        <v>0.05199411883950233</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.04723206162452698</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -590,7 +673,13 @@
         <v>0.7556673739166735</v>
       </c>
       <c r="C15" t="n">
-        <v>0.6791902065932923</v>
+        <v>0.6791952460002608</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.07539159804582596</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.05160433799028397</v>
       </c>
     </row>
     <row r="16">
@@ -603,6 +692,12 @@
       <c r="C16" t="n">
         <v>0.8485848351162421</v>
       </c>
+      <c r="D16" t="n">
+        <v>0.08692525327205658</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.02815583720803261</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -614,6 +709,12 @@
       <c r="C17" t="n">
         <v>0.6481435512895773</v>
       </c>
+      <c r="D17" t="n">
+        <v>0.04295807331800461</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.03566687181591988</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -623,7 +724,13 @@
         <v>0.736135897052708</v>
       </c>
       <c r="C18" t="n">
-        <v>0.6392438152031136</v>
+        <v>0.6392438678374194</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.2073389887809753</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.07804397493600845</v>
       </c>
     </row>
     <row r="19">
@@ -635,6 +742,12 @@
       </c>
       <c r="C19" t="n">
         <v>0.6552475367373298</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.03760791569948196</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.05074924603104591</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added comparison tensorflow and arcface
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -414,7 +414,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C19"/>
+  <dimension ref="A1:E19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -430,12 +430,17 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>Расстояние до переноса стиля</t>
+          <t>Расстояние до переноса стиля tensorflow</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>Расстояние после переноса стиля</t>
+          <t>Расстояние после переноса стиля tensorflow</t>
+        </is>
+      </c>
+      <c r="D1" t="inlineStr">
+        <is>
+          <t>Расстояние до переноса стиля arcface,Расстояние после переноса стиля arcface</t>
         </is>
       </c>
     </row>
@@ -449,6 +454,12 @@
       <c r="C2" t="n">
         <v>0.6900906099731764</v>
       </c>
+      <c r="D2" t="n">
+        <v>0.03230053186416626</v>
+      </c>
+      <c r="E2" t="n">
+        <v>0.01071752980351448</v>
+      </c>
     </row>
     <row r="3">
       <c r="A3" t="n">
@@ -460,6 +471,12 @@
       <c r="C3" t="n">
         <v>0.8114843020131262</v>
       </c>
+      <c r="D3" t="n">
+        <v>0.07159358263015747</v>
+      </c>
+      <c r="E3" t="n">
+        <v>0.06596450507640839</v>
+      </c>
     </row>
     <row r="4">
       <c r="A4" t="n">
@@ -471,6 +488,12 @@
       <c r="C4" t="n">
         <v>0.6384303963590946</v>
       </c>
+      <c r="D4" t="n">
+        <v>0.1831206232309341</v>
+      </c>
+      <c r="E4" t="n">
+        <v>0.01908320561051369</v>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="n">
@@ -480,7 +503,13 @@
         <v>0.7718901967512342</v>
       </c>
       <c r="C5" t="n">
-        <v>0.7964303098175904</v>
+        <v>0.7964307258438679</v>
+      </c>
+      <c r="D5" t="n">
+        <v>0.11044642329216</v>
+      </c>
+      <c r="E5" t="n">
+        <v>0.03032833524048328</v>
       </c>
     </row>
     <row r="6">
@@ -493,6 +522,12 @@
       <c r="C6" t="n">
         <v>0.6163731154104217</v>
       </c>
+      <c r="D6" t="n">
+        <v>0.05190222710371017</v>
+      </c>
+      <c r="E6" t="n">
+        <v>0.06330510973930359</v>
+      </c>
     </row>
     <row r="7">
       <c r="A7" t="n">
@@ -504,6 +539,12 @@
       <c r="C7" t="n">
         <v>0.6820363932821293</v>
       </c>
+      <c r="D7" t="n">
+        <v>0.0741061195731163</v>
+      </c>
+      <c r="E7" t="n">
+        <v>0.0427030511200428</v>
+      </c>
     </row>
     <row r="8">
       <c r="A8" t="n">
@@ -515,6 +556,12 @@
       <c r="C8" t="n">
         <v>0.6573289094154495</v>
       </c>
+      <c r="D8" t="n">
+        <v>0.06903903931379318</v>
+      </c>
+      <c r="E8" t="n">
+        <v>0.04660750180482864</v>
+      </c>
     </row>
     <row r="9">
       <c r="A9" t="n">
@@ -526,6 +573,12 @@
       <c r="C9" t="n">
         <v>0.5903696824065264</v>
       </c>
+      <c r="D9" t="n">
+        <v>0.05451708287000656</v>
+      </c>
+      <c r="E9" t="n">
+        <v>0.03171984478831291</v>
+      </c>
     </row>
     <row r="10">
       <c r="A10" t="n">
@@ -535,7 +588,13 @@
         <v>0.7669342175270629</v>
       </c>
       <c r="C10" t="n">
-        <v>0.7330400849497321</v>
+        <v>0.7330427481233784</v>
+      </c>
+      <c r="D10" t="n">
+        <v>0.1547363102436066</v>
+      </c>
+      <c r="E10" t="n">
+        <v>0.08104228973388672</v>
       </c>
     </row>
     <row r="11">
@@ -546,7 +605,13 @@
         <v>0.7950532845299012</v>
       </c>
       <c r="C11" t="n">
-        <v>0.754820729126691</v>
+        <v>0.754825674803941</v>
+      </c>
+      <c r="D11" t="n">
+        <v>0.04635890573263168</v>
+      </c>
+      <c r="E11" t="n">
+        <v>0.06895835697650909</v>
       </c>
     </row>
     <row r="12">
@@ -557,7 +622,13 @@
         <v>0.4914829060884561</v>
       </c>
       <c r="C12" t="n">
-        <v>0.4725797102277756</v>
+        <v>0.4725813935492413</v>
+      </c>
+      <c r="D12" t="n">
+        <v>0.01744678616523743</v>
+      </c>
+      <c r="E12" t="n">
+        <v>0.02074667811393738</v>
       </c>
     </row>
     <row r="13">
@@ -570,6 +641,12 @@
       <c r="C13" t="n">
         <v>0.6552857113411387</v>
       </c>
+      <c r="D13" t="n">
+        <v>0.03705150634050369</v>
+      </c>
+      <c r="E13" t="n">
+        <v>0.02712763473391533</v>
+      </c>
     </row>
     <row r="14">
       <c r="A14" t="n">
@@ -581,6 +658,12 @@
       <c r="C14" t="n">
         <v>0.7545523635001893</v>
       </c>
+      <c r="D14" t="n">
+        <v>0.05199411883950233</v>
+      </c>
+      <c r="E14" t="n">
+        <v>0.04723206162452698</v>
+      </c>
     </row>
     <row r="15">
       <c r="A15" t="n">
@@ -590,7 +673,13 @@
         <v>0.7556673739166735</v>
       </c>
       <c r="C15" t="n">
-        <v>0.6791902065932923</v>
+        <v>0.6791952460002608</v>
+      </c>
+      <c r="D15" t="n">
+        <v>0.07539159804582596</v>
+      </c>
+      <c r="E15" t="n">
+        <v>0.05160433799028397</v>
       </c>
     </row>
     <row r="16">
@@ -603,6 +692,12 @@
       <c r="C16" t="n">
         <v>0.8485848351162421</v>
       </c>
+      <c r="D16" t="n">
+        <v>0.08692525327205658</v>
+      </c>
+      <c r="E16" t="n">
+        <v>0.02815583720803261</v>
+      </c>
     </row>
     <row r="17">
       <c r="A17" t="n">
@@ -614,6 +709,12 @@
       <c r="C17" t="n">
         <v>0.6481435512895773</v>
       </c>
+      <c r="D17" t="n">
+        <v>0.04295807331800461</v>
+      </c>
+      <c r="E17" t="n">
+        <v>0.03566687181591988</v>
+      </c>
     </row>
     <row r="18">
       <c r="A18" t="n">
@@ -623,7 +724,13 @@
         <v>0.736135897052708</v>
       </c>
       <c r="C18" t="n">
-        <v>0.6392438152031136</v>
+        <v>0.6392438678374194</v>
+      </c>
+      <c r="D18" t="n">
+        <v>0.2073389887809753</v>
+      </c>
+      <c r="E18" t="n">
+        <v>0.07804397493600845</v>
       </c>
     </row>
     <row r="19">
@@ -635,6 +742,12 @@
       </c>
       <c r="C19" t="n">
         <v>0.6552475367373298</v>
+      </c>
+      <c r="D19" t="n">
+        <v>0.03760791569948196</v>
+      </c>
+      <c r="E19" t="n">
+        <v>0.05074924603104591</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
changed the embedding calculation when conducting an experiment with style transfer for arcface
</commit_message>
<xml_diff>
--- a/results/results.xlsx
+++ b/results/results.xlsx
@@ -440,7 +440,12 @@
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>Расстояние до переноса стиля arcface,Расстояние после переноса стиля arcface</t>
+          <t>Расстояние до переноса стиля arcface</t>
+        </is>
+      </c>
+      <c r="E1" t="inlineStr">
+        <is>
+          <t>Расстояние после переноса стиля arcface</t>
         </is>
       </c>
     </row>
@@ -452,13 +457,13 @@
         <v>0.6981427289321528</v>
       </c>
       <c r="C2" t="n">
-        <v>0.6900906099731764</v>
+        <v>0.6900752004639339</v>
       </c>
       <c r="D2" t="n">
-        <v>0.03230053186416626</v>
+        <v>0.008492808789014816</v>
       </c>
       <c r="E2" t="n">
-        <v>0.01071752980351448</v>
+        <v>0.002082576043903828</v>
       </c>
     </row>
     <row r="3">
@@ -472,10 +477,10 @@
         <v>0.8114843020131262</v>
       </c>
       <c r="D3" t="n">
-        <v>0.07159358263015747</v>
+        <v>0.01410352624952793</v>
       </c>
       <c r="E3" t="n">
-        <v>0.06596450507640839</v>
+        <v>0.01060810126364231</v>
       </c>
     </row>
     <row r="4">
@@ -489,10 +494,10 @@
         <v>0.6384303963590946</v>
       </c>
       <c r="D4" t="n">
-        <v>0.1831206232309341</v>
+        <v>0.01806437224149704</v>
       </c>
       <c r="E4" t="n">
-        <v>0.01908320561051369</v>
+        <v>0.003665033960714936</v>
       </c>
     </row>
     <row r="5">
@@ -503,13 +508,13 @@
         <v>0.7718901967512342</v>
       </c>
       <c r="C5" t="n">
-        <v>0.7964307258438679</v>
+        <v>0.7964303098175904</v>
       </c>
       <c r="D5" t="n">
-        <v>0.11044642329216</v>
+        <v>0.009923557750880718</v>
       </c>
       <c r="E5" t="n">
-        <v>0.03032833524048328</v>
+        <v>0.005861029028892517</v>
       </c>
     </row>
     <row r="6">
@@ -523,10 +528,10 @@
         <v>0.6163731154104217</v>
       </c>
       <c r="D6" t="n">
-        <v>0.05190222710371017</v>
+        <v>0.01835355162620544</v>
       </c>
       <c r="E6" t="n">
-        <v>0.06330510973930359</v>
+        <v>0.01003515347838402</v>
       </c>
     </row>
     <row r="7">
@@ -540,10 +545,10 @@
         <v>0.6820363932821293</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0741061195731163</v>
+        <v>0.01772580668330193</v>
       </c>
       <c r="E7" t="n">
-        <v>0.0427030511200428</v>
+        <v>0.01566718332469463</v>
       </c>
     </row>
     <row r="8">
@@ -557,10 +562,10 @@
         <v>0.6573289094154495</v>
       </c>
       <c r="D8" t="n">
-        <v>0.06903903931379318</v>
+        <v>0.01674813218414783</v>
       </c>
       <c r="E8" t="n">
-        <v>0.04660750180482864</v>
+        <v>0.00910513661801815</v>
       </c>
     </row>
     <row r="9">
@@ -574,10 +579,10 @@
         <v>0.5903696824065264</v>
       </c>
       <c r="D9" t="n">
-        <v>0.05451708287000656</v>
+        <v>0.02624757029116154</v>
       </c>
       <c r="E9" t="n">
-        <v>0.03171984478831291</v>
+        <v>0.01961797103285789</v>
       </c>
     </row>
     <row r="10">
@@ -588,13 +593,13 @@
         <v>0.7669342175270629</v>
       </c>
       <c r="C10" t="n">
-        <v>0.7330427481233784</v>
+        <v>0.7330400849497321</v>
       </c>
       <c r="D10" t="n">
-        <v>0.1547363102436066</v>
+        <v>0.0465083047747612</v>
       </c>
       <c r="E10" t="n">
-        <v>0.08104228973388672</v>
+        <v>0.03962106630206108</v>
       </c>
     </row>
     <row r="11">
@@ -605,13 +610,13 @@
         <v>0.7950532845299012</v>
       </c>
       <c r="C11" t="n">
-        <v>0.754825674803941</v>
+        <v>0.754820729126691</v>
       </c>
       <c r="D11" t="n">
-        <v>0.04635890573263168</v>
+        <v>0.02004562132060528</v>
       </c>
       <c r="E11" t="n">
-        <v>0.06895835697650909</v>
+        <v>0.01289359852671623</v>
       </c>
     </row>
     <row r="12">
@@ -622,13 +627,13 @@
         <v>0.4914829060884561</v>
       </c>
       <c r="C12" t="n">
-        <v>0.4725813935492413</v>
+        <v>0.4725797102277756</v>
       </c>
       <c r="D12" t="n">
-        <v>0.01744678616523743</v>
+        <v>0.006884787697345018</v>
       </c>
       <c r="E12" t="n">
-        <v>0.02074667811393738</v>
+        <v>0.005170291755348444</v>
       </c>
     </row>
     <row r="13">
@@ -642,10 +647,10 @@
         <v>0.6552857113411387</v>
       </c>
       <c r="D13" t="n">
-        <v>0.03705150634050369</v>
+        <v>0.0232948437333107</v>
       </c>
       <c r="E13" t="n">
-        <v>0.02712763473391533</v>
+        <v>0.01254448667168617</v>
       </c>
     </row>
     <row r="14">
@@ -659,10 +664,10 @@
         <v>0.7545523635001893</v>
       </c>
       <c r="D14" t="n">
-        <v>0.05199411883950233</v>
+        <v>0.02751919999718666</v>
       </c>
       <c r="E14" t="n">
-        <v>0.04723206162452698</v>
+        <v>0.02013404667377472</v>
       </c>
     </row>
     <row r="15">
@@ -673,13 +678,13 @@
         <v>0.7556673739166735</v>
       </c>
       <c r="C15" t="n">
-        <v>0.6791952460002608</v>
+        <v>0.6791948264882282</v>
       </c>
       <c r="D15" t="n">
-        <v>0.07539159804582596</v>
+        <v>0.03104481101036072</v>
       </c>
       <c r="E15" t="n">
-        <v>0.05160433799028397</v>
+        <v>0.01083913818001747</v>
       </c>
     </row>
     <row r="16">
@@ -693,10 +698,10 @@
         <v>0.8485848351162421</v>
       </c>
       <c r="D16" t="n">
-        <v>0.08692525327205658</v>
+        <v>0.02553591132164001</v>
       </c>
       <c r="E16" t="n">
-        <v>0.02815583720803261</v>
+        <v>0.01203899551182985</v>
       </c>
     </row>
     <row r="17">
@@ -710,10 +715,10 @@
         <v>0.6481435512895773</v>
       </c>
       <c r="D17" t="n">
-        <v>0.04295807331800461</v>
+        <v>0.01383387669920921</v>
       </c>
       <c r="E17" t="n">
-        <v>0.03566687181591988</v>
+        <v>0.01148590538650751</v>
       </c>
     </row>
     <row r="18">
@@ -724,13 +729,13 @@
         <v>0.736135897052708</v>
       </c>
       <c r="C18" t="n">
-        <v>0.6392438678374194</v>
+        <v>0.6392436588714024</v>
       </c>
       <c r="D18" t="n">
-        <v>0.2073389887809753</v>
+        <v>0.1120398044586182</v>
       </c>
       <c r="E18" t="n">
-        <v>0.07804397493600845</v>
+        <v>0.07538660615682602</v>
       </c>
     </row>
     <row r="19">
@@ -741,13 +746,13 @@
         <v>0.7391632763897428</v>
       </c>
       <c r="C19" t="n">
-        <v>0.6552475367373298</v>
+        <v>0.6552471888204152</v>
       </c>
       <c r="D19" t="n">
-        <v>0.03760791569948196</v>
+        <v>0.02931328490376472</v>
       </c>
       <c r="E19" t="n">
-        <v>0.05074924603104591</v>
+        <v>0.02313164621591568</v>
       </c>
     </row>
   </sheetData>

</xml_diff>